<commit_message>
db and tables created
</commit_message>
<xml_diff>
--- a/Test and Test Automation(March 25).xlsx
+++ b/Test and Test Automation(March 25).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\python\LaunchEmployees\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB8A9E0E-9289-4905-86B3-D6F88AEF2658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C3D658-DE6C-4B4A-99F3-A76029A49149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5E500EA5-2953-4230-BF7D-A1621410B6E1}"/>
   </bookViews>
@@ -1211,8 +1211,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1220,14 +1220,14 @@
     <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6328125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="27.54296875" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="19" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="53.453125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="32.08984375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="23.1796875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="34.08984375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1796875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6328125" customWidth="1"/>
+    <col min="5" max="5" width="27.54296875" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="53.453125" customWidth="1"/>
+    <col min="8" max="8" width="32.08984375" customWidth="1"/>
+    <col min="9" max="9" width="23.1796875" customWidth="1"/>
+    <col min="10" max="10" width="34.08984375" customWidth="1"/>
+    <col min="11" max="11" width="10.1796875" customWidth="1"/>
     <col min="12" max="12" width="39.90625" customWidth="1"/>
     <col min="13" max="13" width="22.81640625" customWidth="1"/>
     <col min="14" max="14" width="27.26953125" customWidth="1"/>
@@ -3413,5 +3413,6 @@
     <sortCondition ref="L2:L45"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>